<commit_message>
Chore: reverted reaction to fixedExchange in methionine model
</commit_message>
<xml_diff>
--- a/io/input/methionine_cycle.xlsx
+++ b/io/input/methionine_cycle.xlsx
@@ -505,7 +505,7 @@
     <t xml:space="preserve">nadph binds first and mthf is the second product</t>
   </si>
   <si>
-    <t xml:space="preserve">massAction</t>
+    <t xml:space="preserve">fixedExchange</t>
   </si>
   <si>
     <t xml:space="preserve">This reaction describes the methionine intake</t>
@@ -903,7 +903,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2888,14 +2888,14 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="3.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="4.1"/>
@@ -4291,7 +4291,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Tests: updated unit tests
</commit_message>
<xml_diff>
--- a/io/input/methionine_cycle.xlsx
+++ b/io/input/methionine_cycle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -755,8 +755,8 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -873,7 +873,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2531,8 +2531,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
chore: Remove measured? column from mets sheet
It was not used anywhere.
</commit_message>
<xml_diff>
--- a/io/input/methionine_cycle.xlsx
+++ b/io/input/methionine_cycle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="152">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t xml:space="preserve">balanced?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">measured?</t>
   </si>
   <si>
     <t xml:space="preserve">methionine</t>
@@ -650,11 +647,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -733,7 +730,7 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -879,32 +876,32 @@
   </cols>
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>103</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,66 +1307,66 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="18" t="s">
         <v>110</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="10" t="n">
+      <c r="B2" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="C2" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="10" t="n">
+      <c r="C2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="E2" s="10" t="n">
+      <c r="E2" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="F2" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="10" t="n">
+      <c r="F2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="I2" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="10" t="n">
+      <c r="I2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1377,31 +1374,31 @@
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="10" t="n">
+      <c r="B3" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="C3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10" t="n">
+      <c r="C3" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="E3" s="10" t="n">
+      <c r="E3" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="F3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="10" t="n">
+      <c r="F3" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="H3" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="I3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="10" t="n">
+      <c r="I3" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1409,31 +1406,31 @@
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="10" t="n">
+      <c r="B4" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="C4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10" t="n">
+      <c r="C4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="E4" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="F4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="10" t="n">
+      <c r="F4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="H4" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="I4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="10" t="n">
+      <c r="I4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1441,31 +1438,31 @@
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="10" t="n">
+      <c r="B5" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="C5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10" t="n">
+      <c r="C5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="E5" s="10" t="n">
+      <c r="E5" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="F5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="10" t="n">
+      <c r="F5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="H5" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="I5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="10" t="n">
+      <c r="I5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1473,31 +1470,31 @@
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="10" t="n">
+      <c r="B6" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="C6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="10" t="n">
+      <c r="C6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="E6" s="10" t="n">
+      <c r="E6" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="F6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="10" t="n">
+      <c r="F6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="H6" s="10" t="n">
+      <c r="H6" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="I6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="10" t="n">
+      <c r="I6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1505,31 +1502,31 @@
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="10" t="n">
+      <c r="B7" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="C7" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="10" t="n">
+      <c r="C7" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="E7" s="10" t="n">
+      <c r="E7" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="F7" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="10" t="n">
+      <c r="F7" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="H7" s="10" t="n">
+      <c r="H7" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="I7" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="10" t="n">
+      <c r="I7" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="9" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1537,31 +1534,31 @@
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="10" t="n">
+      <c r="B8" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="C8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="10" t="n">
+      <c r="C8" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="E8" s="10" t="n">
+      <c r="E8" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="F8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="10" t="n">
+      <c r="F8" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="H8" s="10" t="n">
+      <c r="H8" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="I8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="10" t="n">
+      <c r="I8" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="9" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1569,31 +1566,31 @@
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="10" t="n">
+      <c r="B9" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="C9" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="10" t="n">
+      <c r="C9" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="E9" s="10" t="n">
+      <c r="E9" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="F9" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="10" t="n">
+      <c r="F9" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="H9" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="10" t="n">
+      <c r="H9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1601,31 +1598,31 @@
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="10" t="n">
+      <c r="B10" s="9" t="n">
         <v>1.5</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="9" t="n">
         <v>1.5</v>
       </c>
-      <c r="D10" s="10" t="n">
+      <c r="D10" s="9" t="n">
         <v>1.5</v>
       </c>
-      <c r="E10" s="10" t="n">
+      <c r="E10" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="F10" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="10" t="n">
+      <c r="F10" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="H10" s="10" t="n">
+      <c r="H10" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="I10" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="10" t="n">
+      <c r="I10" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="9" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1633,31 +1630,31 @@
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="10" t="n">
+      <c r="B11" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="C11" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="10" t="n">
+      <c r="C11" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="E11" s="10" t="n">
+      <c r="E11" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="F11" s="10" t="n">
+      <c r="F11" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="G11" s="10" t="n">
+      <c r="G11" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="H11" s="10" t="n">
+      <c r="H11" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="I11" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="10" t="n">
+      <c r="I11" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="9" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1665,31 +1662,31 @@
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="10" t="n">
+      <c r="B12" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="C12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="10" t="n">
+      <c r="C12" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="E12" s="10" t="n">
+      <c r="E12" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="F12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="10" t="n">
+      <c r="F12" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9" t="n">
         <v>1.01</v>
       </c>
-      <c r="H12" s="10" t="n">
+      <c r="H12" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="I12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="10" t="n">
+      <c r="I12" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="9" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1735,35 +1732,35 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="18" t="s">
         <v>110</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,41 +2507,41 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2552,7 +2549,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -2572,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,10 +2577,10 @@
         <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>125</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>126</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>20</v>
@@ -2600,7 +2597,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2608,10 +2605,10 @@
         <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>125</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>126</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>20</v>
@@ -2626,7 +2623,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2634,13 +2631,13 @@
         <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="D5" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>26</v>
@@ -2652,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,13 +2657,13 @@
         <v>43</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="D6" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>134</v>
       </c>
       <c r="J6" s="1" t="n">
         <v>1</v>
@@ -2675,7 +2672,7 @@
         <v>4</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2683,22 +2680,22 @@
         <v>44</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="24" t="s">
         <v>137</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2706,22 +2703,22 @@
         <v>45</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="J8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2729,22 +2726,22 @@
         <v>46</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C9" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="J9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="24" t="s">
         <v>143</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2752,10 +2749,10 @@
         <v>47</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>31</v>
@@ -2770,7 +2767,7 @@
         <v>2</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2778,13 +2775,13 @@
         <v>48</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="D11" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>20</v>
@@ -2796,7 +2793,7 @@
         <v>2</v>
       </c>
       <c r="L11" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2804,7 +2801,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2820,7 +2817,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3744,9 +3741,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -3755,11 +3752,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="11.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="30.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="8.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1010" min="6" style="0" width="8.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="1011" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1009" min="5" style="0" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1018" min="1010" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3772,9 +3768,6 @@
       <c r="C1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -3786,22 +3779,16 @@
       <c r="C2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3809,13 +3796,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3823,13 +3807,10 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3837,12 +3818,9 @@
         <v>21</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3851,87 +3829,69 @@
         <v>22</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="10"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="10"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3945,21 +3905,15 @@
       <c r="C13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D13" s="1" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3968,12 +3922,9 @@
         <v>30</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3982,12 +3933,9 @@
         <v>31</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3996,12 +3944,9 @@
         <v>32</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4010,12 +3955,9 @@
         <v>33</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4024,12 +3966,9 @@
         <v>34</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4043,9 +3982,6 @@
       <c r="C20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="1" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
@@ -4057,21 +3993,15 @@
       <c r="C21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D21" s="1" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4080,12 +4010,9 @@
         <v>38</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4123,16 +4050,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4140,7 +4067,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="7" t="n">
         <v>0</v>
@@ -4151,7 +4078,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="7" t="n">
         <v>0</v>
@@ -4162,7 +4089,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="7" t="n">
         <v>0</v>
@@ -4173,7 +4100,7 @@
         <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="7" t="n">
         <v>0</v>
@@ -4184,7 +4111,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="7" t="n">
         <v>0</v>
@@ -4195,7 +4122,7 @@
         <v>44</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="7" t="n">
         <v>0</v>
@@ -4206,7 +4133,7 @@
         <v>45</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="7" t="n">
         <v>0</v>
@@ -4217,7 +4144,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="7" t="n">
         <v>0</v>
@@ -4228,7 +4155,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="7" t="n">
         <v>0</v>
@@ -4239,7 +4166,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="7" t="n">
         <v>0</v>
@@ -4250,7 +4177,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="7" t="n">
         <v>1</v>
@@ -4289,19 +4216,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4406,14 +4333,14 @@
       <c r="A1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4450,7 +4377,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -4458,7 +4385,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -4581,14 +4508,14 @@
       <c r="A1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4613,12 +4540,12 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4733,13 +4660,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4899,10 +4826,10 @@
         <v>50</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4984,7 +4911,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="16" t="n">
         <v>0.001</v>
@@ -5006,7 +4933,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="17" t="n">
         <v>0.001</v>

</xml_diff>

<commit_message>
fix: Fix thermoRxns bounds in methionine model
</commit_message>
<xml_diff>
--- a/io/input/methionine_cycle.xlsx
+++ b/io/input/methionine_cycle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -735,7 +735,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -875,7 +875,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="B7 H9"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1297,7 +1297,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L32" activeCellId="1" sqref="B7 L32"/>
+      <selection pane="topLeft" activeCell="L32" activeCellId="0" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2068,13 +2068,13 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="B7 B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="9.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="33.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="10.99"/>
@@ -2421,7 +2421,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="B7 A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2434,7 +2434,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="7.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="8" width="3.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="8" width="3.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="8" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="8" width="3.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.84"/>
@@ -2442,7 +2442,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="3.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="3.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="4.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="5.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="3.16"/>
@@ -3321,7 +3321,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B7 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3611,7 +3611,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B7 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3778,7 +3778,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B7 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3952,7 +3952,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="B7 A17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4104,8 +4104,8 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="B7 C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4132,10 +4132,10 @@
         <v>42</v>
       </c>
       <c r="B2" s="13" t="n">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="C2" s="13" t="n">
-        <v>-50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4267,7 +4267,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="1" sqref="B7 A23"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4550,7 +4550,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="B7 B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>